<commit_message>
Beginning heuristic risk assessment and reading data from victim device
</commit_message>
<xml_diff>
--- a/Permission Stats.xlsx
+++ b/Permission Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Graduation-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3BED62-F69C-4978-8804-82288298D626}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F7EA3-280B-49A3-B654-E4236EF9C9C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="791" firstSheet="2" activeTab="5" xr2:uid="{BD4AB7C3-B4B0-443E-94FF-7E4EBBAEED08}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="958" activeTab="3" xr2:uid="{BD4AB7C3-B4B0-443E-94FF-7E4EBBAEED08}"/>
   </bookViews>
   <sheets>
     <sheet name="Permissions by Type and Count" sheetId="1" r:id="rId1"/>
@@ -824,7 +824,112 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="145">
+  <dxfs count="160">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2159,7 +2264,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F1:I1048576"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5841,53 +5946,53 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576 B1:B22 B24:B85 B87:B1048576">
-    <cfRule type="containsText" dxfId="144" priority="11" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="159" priority="11" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="12" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="158" priority="12" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="13" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="157" priority="13" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="14" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="156" priority="14" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="15" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="155" priority="15" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="139" priority="6" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="154" priority="6" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="7" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="153" priority="7" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="8" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="152" priority="8" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="9" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="151" priority="9" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="10" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="150" priority="10" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="containsText" dxfId="134" priority="1" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="149" priority="1" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="2" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="148" priority="2" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="3" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="147" priority="3" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="4" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="146" priority="4" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="5" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="145" priority="5" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B86)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9586,70 +9691,70 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B22 B24:B85 B87:B1048576">
-    <cfRule type="containsText" dxfId="79" priority="16" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="17" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="18" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="19" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="20" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="90" priority="20" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="74" priority="11" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="89" priority="11" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="12" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="88" priority="12" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="13" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="87" priority="13" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="14" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="86" priority="14" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="15" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="85" priority="15" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="containsText" dxfId="69" priority="6" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="84" priority="6" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="8" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="82" priority="8" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="9" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="81" priority="9" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="10" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="64" priority="1" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="79" priority="1" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="78" priority="2" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="77" priority="3" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="76" priority="4" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="75" priority="5" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13347,70 +13452,70 @@
     <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B22 B24:B85 B87:B1048576">
-    <cfRule type="containsText" dxfId="59" priority="16" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="74" priority="16" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="17" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="73" priority="17" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="18" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="72" priority="18" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="19" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="71" priority="19" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="20" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="70" priority="20" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="54" priority="11" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="69" priority="11" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="12" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="68" priority="12" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="67" priority="13" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="14" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="66" priority="14" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="15" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="65" priority="15" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="containsText" dxfId="49" priority="6" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="64" priority="6" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="7" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="63" priority="7" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="8" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="62" priority="8" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="9" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="61" priority="9" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",B86)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="10" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="60" priority="10" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",B86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="44" priority="1" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="2" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="3" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="4" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="56" priority="4" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",G1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="5" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13422,8 +13527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5930FEDB-987C-4F5F-B91F-0CAEB1F465E1}">
   <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P27" sqref="M1:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13439,7 +13544,8 @@
     <col min="9" max="9" width="10.7109375" style="5" customWidth="1"/>
     <col min="10" max="10" width="46" style="5" customWidth="1"/>
     <col min="11" max="11" width="6.42578125" style="5" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="5"/>
+    <col min="16" max="16" width="18.28515625" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -13460,7 +13566,7 @@
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
     </row>
@@ -13494,7 +13600,7 @@
         <v>0.15</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
     </row>
@@ -13528,7 +13634,7 @@
         <v>0.1</v>
       </c>
       <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
     </row>
@@ -13562,7 +13668,7 @@
         <v>0.05</v>
       </c>
       <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
     </row>
@@ -13596,7 +13702,7 @@
         <v>0.3</v>
       </c>
       <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
     </row>
@@ -13630,7 +13736,7 @@
         <v>0.25</v>
       </c>
       <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
     </row>
@@ -13664,7 +13770,7 @@
         <v>0.2</v>
       </c>
       <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
     </row>
@@ -13698,7 +13804,7 @@
         <v>0.15</v>
       </c>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
     </row>
@@ -13732,7 +13838,7 @@
         <v>0.15</v>
       </c>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
     </row>
@@ -13766,7 +13872,7 @@
         <v>0.1</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
     </row>
@@ -13800,7 +13906,7 @@
         <v>0.1</v>
       </c>
       <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="M11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
@@ -13834,7 +13940,7 @@
         <v>0.05</v>
       </c>
       <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
@@ -13868,7 +13974,7 @@
         <v>0.05</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
     </row>
@@ -13902,7 +14008,7 @@
         <v>0.05</v>
       </c>
       <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
@@ -13936,7 +14042,7 @@
         <v>0.4</v>
       </c>
       <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
+      <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
@@ -13970,7 +14076,7 @@
         <v>0.4</v>
       </c>
       <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
+      <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
     </row>
@@ -14004,7 +14110,7 @@
         <v>0.35</v>
       </c>
       <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
+      <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
@@ -14038,9 +14144,9 @@
         <v>0.35</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="11"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -14072,9 +14178,9 @@
         <v>0.35</v>
       </c>
       <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="11"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="9"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -14106,9 +14212,9 @@
         <v>0.3</v>
       </c>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="11"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -14140,9 +14246,9 @@
         <v>0.25</v>
       </c>
       <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="11"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -14174,9 +14280,9 @@
         <v>0.2</v>
       </c>
       <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="11"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="9"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -14208,9 +14314,9 @@
         <v>0.2</v>
       </c>
       <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
+      <c r="M23" s="7"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
+      <c r="O23" s="9"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -14242,9 +14348,9 @@
         <v>0.2</v>
       </c>
       <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
+      <c r="M24" s="11"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -14276,9 +14382,9 @@
         <v>0.15</v>
       </c>
       <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
+      <c r="M25" s="11"/>
       <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
+      <c r="O25" s="10"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -14310,9 +14416,9 @@
         <v>0.15</v>
       </c>
       <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="10"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -16474,71 +16580,71 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576 E1:E1048576 I1:I1048576">
-    <cfRule type="containsText" dxfId="109" priority="16" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="124" priority="31" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="17" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="123" priority="32" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="18" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="122" priority="33" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="19" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="121" priority="34" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="20" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="120" priority="35" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N17">
-    <cfRule type="containsText" dxfId="104" priority="11" operator="containsText" text="other">
-      <formula>NOT(ISERROR(SEARCH("other",N1)))</formula>
+  <conditionalFormatting sqref="M1:M17">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="other">
+      <formula>NOT(ISERROR(SEARCH("other",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="12" operator="containsText" text="signature">
-      <formula>NOT(ISERROR(SEARCH("signature",N1)))</formula>
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="signature">
+      <formula>NOT(ISERROR(SEARCH("signature",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="13" operator="containsText" text="removed">
-      <formula>NOT(ISERROR(SEARCH("removed",N1)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="removed">
+      <formula>NOT(ISERROR(SEARCH("removed",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="14" operator="containsText" text="normal">
-      <formula>NOT(ISERROR(SEARCH("normal",N1)))</formula>
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="normal">
+      <formula>NOT(ISERROR(SEARCH("normal",M1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="15" operator="containsText" text="dangerous">
-      <formula>NOT(ISERROR(SEARCH("dangerous",N1)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="dangerous">
+      <formula>NOT(ISERROR(SEARCH("dangerous",M1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18:N22">
-    <cfRule type="containsText" dxfId="99" priority="6" operator="containsText" text="other">
-      <formula>NOT(ISERROR(SEARCH("other",N18)))</formula>
+  <conditionalFormatting sqref="M18:M23">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="other">
+      <formula>NOT(ISERROR(SEARCH("other",M18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="7" operator="containsText" text="signature">
-      <formula>NOT(ISERROR(SEARCH("signature",N18)))</formula>
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="signature">
+      <formula>NOT(ISERROR(SEARCH("signature",M18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="removed">
-      <formula>NOT(ISERROR(SEARCH("removed",N18)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="removed">
+      <formula>NOT(ISERROR(SEARCH("removed",M18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="normal">
-      <formula>NOT(ISERROR(SEARCH("normal",N18)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="normal">
+      <formula>NOT(ISERROR(SEARCH("normal",M18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="10" operator="containsText" text="dangerous">
-      <formula>NOT(ISERROR(SEARCH("dangerous",N18)))</formula>
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="dangerous">
+      <formula>NOT(ISERROR(SEARCH("dangerous",M18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N23:N25">
-    <cfRule type="containsText" dxfId="94" priority="1" operator="containsText" text="other">
-      <formula>NOT(ISERROR(SEARCH("other",N23)))</formula>
+  <conditionalFormatting sqref="M24:M26">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="other">
+      <formula>NOT(ISERROR(SEARCH("other",M24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="2" operator="containsText" text="signature">
-      <formula>NOT(ISERROR(SEARCH("signature",N23)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="signature">
+      <formula>NOT(ISERROR(SEARCH("signature",M24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="3" operator="containsText" text="removed">
-      <formula>NOT(ISERROR(SEARCH("removed",N23)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="removed">
+      <formula>NOT(ISERROR(SEARCH("removed",M24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="4" operator="containsText" text="normal">
-      <formula>NOT(ISERROR(SEARCH("normal",N23)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="normal">
+      <formula>NOT(ISERROR(SEARCH("normal",M24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="5" operator="containsText" text="dangerous">
-      <formula>NOT(ISERROR(SEARCH("dangerous",N23)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="dangerous">
+      <formula>NOT(ISERROR(SEARCH("dangerous",M24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19601,70 +19707,70 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576 E1:E1048576 I1:I1048576">
-    <cfRule type="containsText" dxfId="39" priority="16" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="54" priority="16" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="17" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="53" priority="17" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="52" priority="18" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="19" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="51" priority="19" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="20" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="50" priority="20" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N17">
-    <cfRule type="containsText" dxfId="34" priority="11" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="12" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="13" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="47" priority="13" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="46" priority="14" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N22">
-    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="44" priority="6" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="43" priority="7" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="8" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="42" priority="8" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N25">
-    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="38" priority="2" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N23)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19676,8 +19782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4DCDBE-75EE-497B-BAA1-4A666D9F897F}">
   <dimension ref="A1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I1:K1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22728,70 +22834,70 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A1048576 E1:E1048576 I1:I1048576">
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="33" priority="17" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="32" priority="18" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="31" priority="19" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="30" priority="20" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N17">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="29" priority="11" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="28" priority="12" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="27" priority="13" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N22">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="24" priority="6" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23:N25">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="other">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="other">
       <formula>NOT(ISERROR(SEARCH("other",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="signature">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="signature">
       <formula>NOT(ISERROR(SEARCH("signature",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="removed">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="removed">
       <formula>NOT(ISERROR(SEARCH("removed",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="normal">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="normal">
       <formula>NOT(ISERROR(SEARCH("normal",N23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="dangerous">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="dangerous">
       <formula>NOT(ISERROR(SEARCH("dangerous",N23)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>